<commit_message>
Sesión 4 - Notas actualizadas
</commit_message>
<xml_diff>
--- a/laboratorio/lab3.xlsx
+++ b/laboratorio/lab3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Documents/Cursos 2025/BELATRIX-EXCEL/curso/laboratorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B29EB4-58E2-C04E-9C98-9C0C100D357A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CEC88E-0D96-D24A-B05D-42276DCD853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16060" xr2:uid="{4DEAC989-7007-CF40-8197-F630010E57D3}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{4DEAC989-7007-CF40-8197-F630010E57D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>